<commit_message>
App restructured, UI added
</commit_message>
<xml_diff>
--- a/resources/Cohort Metadata.xlsx
+++ b/resources/Cohort Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndidier\Desktop\skyn_data_manager\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50051FA1-3E4C-438E-9A02-F0437CCF3D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB870CFE-9DE5-403E-A4ED-23C891D5B150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1515" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Quality" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="40">
   <si>
     <t>Alc</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>TotalDrks</t>
+  </si>
+  <si>
+    <t>Episode_Identifier</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G196" sqref="G196"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>37</v>

</xml_diff>